<commit_message>
Updated backend and readme
</commit_message>
<xml_diff>
--- a/backend/Gym_Schedule_Output.xlsx
+++ b/backend/Gym_Schedule_Output.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Time Slot</t>
   </si>
@@ -83,43 +83,13 @@
   </si>
   <si>
     <t>5:00 PM - 6:00 PM (Friday)</t>
-  </si>
-  <si>
-    <t>6:30 PM - 8:00 PM (Wednesday)</t>
-  </si>
-  <si>
-    <t>9:00 AM - 11:00 AM (Saturday)</t>
-  </si>
-  <si>
-    <t>Aurora Stars (Basketball Camp)</t>
-  </si>
-  <si>
-    <t>6:00 PM - 7:30 PM (Monday)</t>
-  </si>
-  <si>
-    <t>Freedom Flyers (Junior Basketball)</t>
-  </si>
-  <si>
-    <t>6:00 PM - 7:30 PM (Wednesday)</t>
-  </si>
-  <si>
-    <t>4:00 PM - 5:30 PM (Thursday)</t>
-  </si>
-  <si>
-    <t>Harwood Hawks (Volleyball Practice)</t>
-  </si>
-  <si>
-    <t>7:00 PM - 8:30 PM (Friday)</t>
-  </si>
-  <si>
-    <t>Legacy Lions (Soccer Practice)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -127,16 +97,34 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <color rgb="FFFFFF"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="1F497D"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="4F81BD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE6F1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -144,12 +132,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,149 +494,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:O9"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="15" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K2" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K3" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>30</v>
-      </c>
-      <c r="G14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>32</v>
-      </c>
-      <c r="K15" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>